<commit_message>
repushing the last commit
</commit_message>
<xml_diff>
--- a/analysis/fullData_analysis/survey_analysis/all_survey_results.xlsx
+++ b/analysis/fullData_analysis/survey_analysis/all_survey_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasu1\Code\RTmocapFB\analysis\fullData_analysis\survey_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E22503-8019-4FCD-8F3A-52B55B357667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C08C0F6-6EE3-43B8-BB37-49CD7B101D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29475" yWindow="600" windowWidth="22980" windowHeight="12195" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="Open" sheetId="7" r:id="rId7"/>
     <sheet name="Demograph" sheetId="8" r:id="rId8"/>
     <sheet name="General" sheetId="9" r:id="rId9"/>
-    <sheet name="Coding" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5537" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5424" uniqueCount="369">
   <si>
     <t>id. Response ID</t>
   </si>
@@ -1479,7 +1478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1594,123 +1593,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1756,7 +1638,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1766,36 +1648,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2162,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EJ37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="AG1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14246,476 +14098,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A0FDFA-80F1-4DB9-8670-8647A53E9812}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:D37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="88.2" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="4" width="64" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="320.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="88.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>329</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="35" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19598,8 +18980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20465,7 +19847,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21219,15 +20601,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375"/>
-    <col min="4" max="4" width="235.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24" style="1" customWidth="1"/>
+    <col min="4" max="4" width="153.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -21250,34 +20633,34 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E3" t="s">
@@ -21287,17 +20670,17 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E4" t="s">
@@ -21307,17 +20690,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>158</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E5" t="s">
@@ -21327,42 +20710,42 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>157</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>157</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>158</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E8" t="s">
@@ -21372,17 +20755,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>158</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>201</v>
       </c>
       <c r="E9" t="s">
@@ -21392,31 +20775,31 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>211</v>
       </c>
       <c r="E11" t="s">
@@ -21426,48 +20809,48 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>216</v>
       </c>
       <c r="E12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>221</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E13" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>157</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>226</v>
       </c>
       <c r="E14" t="s">
@@ -21477,17 +20860,17 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>144</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>232</v>
       </c>
       <c r="E15" t="s">
@@ -21497,17 +20880,17 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>157</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>237</v>
       </c>
       <c r="E16" t="s">
@@ -21517,17 +20900,17 @@
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>158</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>246</v>
       </c>
       <c r="E17" t="s">
@@ -21537,31 +20920,31 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>252</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>158</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>257</v>
       </c>
       <c r="E19" t="s">
@@ -21571,45 +20954,45 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>252</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>157</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>271</v>
       </c>
       <c r="E22" t="s">
@@ -21619,14 +21002,14 @@
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>157</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E23" t="s">
@@ -21636,34 +21019,34 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E24" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
         <v>158</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>285</v>
       </c>
       <c r="E25" t="s">
@@ -21673,31 +21056,31 @@
         <v>286</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
       <c r="B26">
         <v>12</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
       <c r="B27" t="s">
         <v>157</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>295</v>
       </c>
       <c r="E27" t="s">
@@ -21707,59 +21090,59 @@
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28" t="s">
         <v>252</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E28" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>157</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E29" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>157</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>301</v>
       </c>
       <c r="E30" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>158</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E31" t="s">
@@ -21769,93 +21152,93 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
       <c r="B32" t="s">
         <v>144</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E32" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>158</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E33" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>221</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
         <v>10</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>317</v>
       </c>
       <c r="E35" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36">
         <v>10</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>322</v>
       </c>
       <c r="E36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
       <c r="B37" t="s">
         <v>221</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>326</v>
       </c>
       <c r="E37" t="s">
@@ -21874,8 +21257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23074,7 +22457,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B37"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="169.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>